<commit_message>
updated feature for backend 4/8/2022
</commit_message>
<xml_diff>
--- a/dcomtestcasegeneration/Document/CA_C385EV_BL02_RC09_ DCOM_Full_VIIIICAMPC-516.xlsx
+++ b/dcomtestcasegeneration/Document/CA_C385EV_BL02_RC09_ DCOM_Full_VIIIICAMPC-516.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BHG81HC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HuyNA_repo\dcomtestcasegeneration\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934B864E-F9F9-4A74-9094-5C17BA82CECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D8CBCC-7799-4B95-ACD5-B493FC921EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26310" yWindow="945" windowWidth="24855" windowHeight="15315" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3E" sheetId="4" r:id="rId1"/>
@@ -20637,7 +20637,7 @@
   <dimension ref="A1:L262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -22943,8 +22943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23579,8 +23579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31501,8 +31501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="C19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31978,8 +31978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -36514,7 +36514,7 @@
   <dimension ref="A1:G275"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39249,8 +39249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -42050,7 +42050,7 @@
   <dimension ref="A1:L270"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -45956,7 +45956,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H4" sqref="H4:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>